<commit_message>
successfuly test drop down menu in shopping websiteä
q

qqq
quit
</commit_message>
<xml_diff>
--- a/Data/drop_down_menu_data.xlsx
+++ b/Data/drop_down_menu_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/venkatabandi/google_backup/ta-sausedemo/ta-sausedemo/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF7FF7A-F5F8-534B-ACC9-5A31DF65E649}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F03EF7E-838A-5541-B917-6825B8252E72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20780" yWindow="5900" windowWidth="27640" windowHeight="16940" xr2:uid="{CCE7BCCA-E375-024A-82F5-620A86C954E8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>$15.99</t>
   </si>
@@ -71,28 +71,10 @@
     <t>Sauce Labs Backpack</t>
   </si>
   <si>
-    <t>${priceZA}</t>
-  </si>
-  <si>
-    <t>${nameZA}</t>
-  </si>
-  <si>
-    <t>${priceAZ}</t>
-  </si>
-  <si>
-    <t>${nameAZ}</t>
-  </si>
-  <si>
-    <t>${priceLH}</t>
-  </si>
-  <si>
-    <t>${nameLH}</t>
-  </si>
-  <si>
-    <t>${priceHL}</t>
-  </si>
-  <si>
-    <t>${nameHL}</t>
+    <t>price</t>
+  </si>
+  <si>
+    <t>name</t>
   </si>
 </sst>
 </file>
@@ -465,200 +447,81 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2495F8F5-4D8C-0E45-8334-69026E6A4647}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="27.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" t="s">
-        <v>0</v>
-      </c>
-      <c r="H4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G5" t="s">
-        <v>0</v>
-      </c>
-      <c r="H5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" t="s">
-        <v>3</v>
-      </c>
-      <c r="H6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G7" t="s">
-        <v>1</v>
-      </c>
-      <c r="H7" t="s">
-        <v>6</v>
-      </c>
+      <c r="D7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>